<commit_message>
corrected popups totally had to replace one image bc it was being entirely too weird next I need to make it interactive so it can page through the DatesBackTo years
</commit_message>
<xml_diff>
--- a/NyckelharpaHistoryData.xlsx
+++ b/NyckelharpaHistoryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720586F3-BCB0-4C2B-9F9E-5DAD2A92F311}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557FD74A-FBD2-4B17-AA1B-415E1BE3C6DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4785" windowWidth="29040" windowHeight="15840" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
   <si>
     <t>InstrumentName</t>
   </si>
@@ -269,18 +269,54 @@
     <t>Localimage</t>
   </si>
   <si>
+    <t>By User:pincopallino - Own work, Public Domain, https://commons.wikimedia.org/w/index.php?curid=3790206</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f3/Strohfiddel.jpg/260px-Strohfiddel.jpg</t>
+  </si>
+  <si>
+    <t>Attribution</t>
+  </si>
+  <si>
+    <t>1350 CE</t>
+  </si>
+  <si>
+    <t>1526 CE</t>
+  </si>
+  <si>
+    <t>1600 CE</t>
+  </si>
+  <si>
+    <t>1630 CE</t>
+  </si>
+  <si>
+    <t>1200 CE</t>
+  </si>
+  <si>
+    <t>1998 CE</t>
+  </si>
+  <si>
+    <t>1408 CE</t>
+  </si>
+  <si>
+    <t>1503 CE</t>
+  </si>
+  <si>
+    <t>1529 CE</t>
+  </si>
+  <si>
+    <t>1619 CE</t>
+  </si>
+  <si>
+    <t>images/kallunge_carving.jpg</t>
+  </si>
+  <si>
+    <t>images/moraharpa.jpg</t>
+  </si>
+  <si>
     <t>images/esse_harpa.jpg</t>
   </si>
   <si>
-    <t>images/moraharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/kallunge_carving.jpg</t>
-  </si>
-  <si>
-    <t>images/vefsen_harpa.jpg</t>
-  </si>
-  <si>
     <t>images/kontrabasharpa.jpg</t>
   </si>
   <si>
@@ -290,9 +326,6 @@
     <t>images/EricSahlstromInstitute.png</t>
   </si>
   <si>
-    <t>By User:pincopallino - Own work, Public Domain, https://commons.wikimedia.org/w/index.php?curid=3790206</t>
-  </si>
-  <si>
     <t>images/Viola_a_chiavi_Siena_1408.jpg</t>
   </si>
   <si>
@@ -302,10 +335,10 @@
     <t>images/Schluesselfidel.jpg</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f3/Strohfiddel.jpg/260px-Strohfiddel.jpg</t>
-  </si>
-  <si>
     <t>images/Strohfiddel.jpg</t>
+  </si>
+  <si>
+    <t>images/vefsen.png</t>
   </si>
 </sst>
 </file>
@@ -694,7 +727,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,6 +764,9 @@
       <c r="H1" t="s">
         <v>77</v>
       </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -745,8 +781,8 @@
       <c r="D2">
         <v>18.568551200000002</v>
       </c>
-      <c r="E2">
-        <v>1350</v>
+      <c r="E2" t="s">
+        <v>81</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
@@ -755,7 +791,7 @@
         <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -771,8 +807,8 @@
       <c r="D3">
         <v>14.482189999999999</v>
       </c>
-      <c r="E3">
-        <v>1526</v>
+      <c r="E3" t="s">
+        <v>82</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -781,7 +817,7 @@
         <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -797,8 +833,8 @@
       <c r="D4">
         <v>13.145485300000001</v>
       </c>
-      <c r="E4">
-        <v>1600</v>
+      <c r="E4" t="s">
+        <v>83</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -807,7 +843,7 @@
         <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -823,8 +859,8 @@
       <c r="D5">
         <v>22.788154500000001</v>
       </c>
-      <c r="E5">
-        <v>1600</v>
+      <c r="E5" t="s">
+        <v>83</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
@@ -833,7 +869,7 @@
         <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -849,8 +885,8 @@
       <c r="D6">
         <v>17.518364699999999</v>
       </c>
-      <c r="E6">
-        <v>1630</v>
+      <c r="E6" t="s">
+        <v>84</v>
       </c>
       <c r="F6" t="s">
         <v>46</v>
@@ -859,7 +895,7 @@
         <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,8 +911,8 @@
       <c r="D7">
         <v>17.688720199999999</v>
       </c>
-      <c r="E7">
-        <v>1200</v>
+      <c r="E7" t="s">
+        <v>85</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -885,7 +921,7 @@
         <v>74</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -901,8 +937,8 @@
       <c r="D8">
         <v>17.6540985</v>
       </c>
-      <c r="E8">
-        <v>1998</v>
+      <c r="E8" t="s">
+        <v>86</v>
       </c>
       <c r="F8" t="s">
         <v>53</v>
@@ -911,7 +947,7 @@
         <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -927,8 +963,8 @@
       <c r="D9">
         <v>11.329836999999999</v>
       </c>
-      <c r="E9">
-        <v>1408</v>
+      <c r="E9" t="s">
+        <v>87</v>
       </c>
       <c r="F9" t="s">
         <v>62</v>
@@ -937,10 +973,10 @@
         <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -956,8 +992,8 @@
       <c r="D10">
         <v>17.484182700000002</v>
       </c>
-      <c r="E10">
-        <v>1503</v>
+      <c r="E10" t="s">
+        <v>88</v>
       </c>
       <c r="F10" t="s">
         <v>65</v>
@@ -966,7 +1002,7 @@
         <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -982,8 +1018,8 @@
       <c r="D11">
         <v>9.8746261000000004</v>
       </c>
-      <c r="E11">
-        <v>1529</v>
+      <c r="E11" t="s">
+        <v>89</v>
       </c>
       <c r="F11" t="s">
         <v>69</v>
@@ -992,7 +1028,7 @@
         <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1008,17 +1044,17 @@
       <c r="D12">
         <v>13.632501599999999</v>
       </c>
-      <c r="E12">
-        <v>1619</v>
+      <c r="E12" t="s">
+        <v>90</v>
       </c>
       <c r="F12" t="s">
         <v>71</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some attributions for images still more to go asked permission to use for the kallunge one
</commit_message>
<xml_diff>
--- a/NyckelharpaHistoryData.xlsx
+++ b/NyckelharpaHistoryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557FD74A-FBD2-4B17-AA1B-415E1BE3C6DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9047A7-189B-4251-817F-EB48EBD2829A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4785" windowWidth="29040" windowHeight="15840" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Geo" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
   <si>
     <t>InstrumentName</t>
   </si>
@@ -200,18 +200,12 @@
     <t>Vefsen harpa now in Musik Museum in Stockholm</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>https://nyckelharpansforum.net/global/piccar/kbhr.jpg</t>
   </si>
   <si>
     <t>https://nyckelharpansforum.net/bildsidor/2000esse.jpg</t>
   </si>
   <si>
-    <t>http://66.media.tumblr.com/tumblr_mdi0itmzmY1qiw9oko1_500.jpg</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Nyckelharpa#/media/File:Viola_a_chiavi_Siena_1408.jpg</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>http://www.nyckelharpa.org/images/large/vefsen_harpa.jpg</t>
   </si>
   <si>
-    <t>https://html2-f.scribdassets.com/6e3otzf8ow5cs6rd/images/2-0def780a97.jpg</t>
-  </si>
-  <si>
     <t>DatesBackTo</t>
   </si>
   <si>
@@ -269,9 +260,6 @@
     <t>Localimage</t>
   </si>
   <si>
-    <t>By User:pincopallino - Own work, Public Domain, https://commons.wikimedia.org/w/index.php?curid=3790206</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/f/f3/Strohfiddel.jpg/260px-Strohfiddel.jpg</t>
   </si>
   <si>
@@ -320,12 +308,6 @@
     <t>images/kontrabasharpa.jpg</t>
   </si>
   <si>
-    <t>images/2-0def780a97.jpg</t>
-  </si>
-  <si>
-    <t>images/EricSahlstromInstitute.png</t>
-  </si>
-  <si>
     <t>images/Viola_a_chiavi_Siena_1408.jpg</t>
   </si>
   <si>
@@ -339,6 +321,30 @@
   </si>
   <si>
     <t>images/vefsen.png</t>
+  </si>
+  <si>
+    <t>Image Source</t>
+  </si>
+  <si>
+    <t>Magnus Holmström</t>
+  </si>
+  <si>
+    <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>images/sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>By User:pincopallino - Own work, Public Domain</t>
+  </si>
+  <si>
+    <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
+  </si>
+  <si>
+    <t>images/ESI.jpg</t>
   </si>
 </sst>
 </file>
@@ -383,11 +389,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -726,17 +733,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C19648A-7D51-4B77-BA95-465F033E890E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="91.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="53.140625" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -753,19 +761,19 @@
         <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,16 +790,16 @@
         <v>18.568551200000002</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -808,16 +816,16 @@
         <v>14.482189999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -834,16 +842,16 @@
         <v>13.145485300000001</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -860,16 +868,16 @@
         <v>22.788154500000001</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,16 +894,16 @@
         <v>17.518364699999999</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,16 +920,19 @@
         <v>17.688720199999999</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>74</v>
+      <c r="G7" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -938,24 +949,24 @@
         <v>17.6540985</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>72</v>
+      <c r="G8" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>43.317990899999998</v>
@@ -964,19 +975,19 @@
         <v>11.329836999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -984,7 +995,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>60.347051299999997</v>
@@ -993,24 +1004,27 @@
         <v>17.484182700000002</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>52.143595900000001</v>
@@ -1019,24 +1033,27 @@
         <v>9.8746261000000004</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="I11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>51.076749999999997</v>
@@ -1045,21 +1062,30 @@
         <v>13.632501599999999</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" location="/media/File:Viola_a_chiavi_Siena_1408.jpg" xr:uid="{13338E98-F238-4A3B-AC5F-65948EC73BF5}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{F6175E98-D11D-4443-959D-0FBAC7D03B22}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{B23186D6-252A-4B93-99F7-350D60FAD10D}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{8F61598F-DCFC-47D8-814E-765D1E3ABD12}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added more images and rows to the data but I need to stop soon bc it's getting to be too much
</commit_message>
<xml_diff>
--- a/NyckelharpaHistoryData.xlsx
+++ b/NyckelharpaHistoryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9047A7-189B-4251-817F-EB48EBD2829A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E229C2-B2D6-4E1B-863F-D0B4907C8B44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
   <si>
     <t>InstrumentName</t>
   </si>
@@ -149,15 +149,9 @@
     <t>Källunge</t>
   </si>
   <si>
-    <t>relief in church</t>
-  </si>
-  <si>
     <t>Mora</t>
   </si>
   <si>
-    <t>actual instrument (Moraharpa)</t>
-  </si>
-  <si>
     <t>Norway</t>
   </si>
   <si>
@@ -167,15 +161,9 @@
     <t>Esse</t>
   </si>
   <si>
-    <t>Esseharpa</t>
-  </si>
-  <si>
     <t>Uppsala</t>
   </si>
   <si>
-    <t>well-documented kontrabasharpa</t>
-  </si>
-  <si>
     <t>Vefsn</t>
   </si>
   <si>
@@ -188,18 +176,12 @@
     <t>Sigtuna</t>
   </si>
   <si>
-    <t>Sigtuna key!</t>
-  </si>
-  <si>
     <t>Tobo</t>
   </si>
   <si>
     <t>Eric Sahlström Institute</t>
   </si>
   <si>
-    <t>Vefsen harpa now in Musik Museum in Stockholm</t>
-  </si>
-  <si>
     <t>https://nyckelharpansforum.net/global/piccar/kbhr.jpg</t>
   </si>
   <si>
@@ -215,18 +197,12 @@
     <t>Siena</t>
   </si>
   <si>
-    <t>Angel on a fresco by Taddeo di Bartolo</t>
-  </si>
-  <si>
     <t>Tierp</t>
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/da/Sweden_tolfta_church_angels_with_nyckelharpa.jpg/800px-Sweden_tolfta_church_angels_with_nyckelharpa.jpg</t>
   </si>
   <si>
-    <t>two angels with nyckelharpa</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -236,18 +212,12 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/8/89/Schluesselfidel_Knochenhaueramtshaus_Hildesheim.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Schlusselfidel </t>
-  </si>
-  <si>
     <t>Dresden</t>
   </si>
   <si>
     <t>Michael Praetorius wrote Syntagma Musicum</t>
   </si>
   <si>
-    <t>http://www.lul.se/Global/Kultur/Nyheter/Bilder/ESI-Tobo-exterior-med-blommor-450pxl.jpg</t>
-  </si>
-  <si>
     <t>http://www.nyckelharpa.org/images/large/vefsen_harpa.jpg</t>
   </si>
   <si>
@@ -345,6 +315,96 @@
   </si>
   <si>
     <t>images/ESI.jpg</t>
+  </si>
+  <si>
+    <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
+  </si>
+  <si>
+    <t>Angel on a fresco on the ceiling of the Palazzo Pubblico (town hall) by Taddeo di Bartolo</t>
+  </si>
+  <si>
+    <t>1830 CE</t>
+  </si>
+  <si>
+    <t>https://olovjohansson.se/nyckelharpa/</t>
+  </si>
+  <si>
+    <t>1498 CE</t>
+  </si>
+  <si>
+    <t>Lagga church outside of Uppsala</t>
+  </si>
+  <si>
+    <t>images/Silverbasharpa.jpg</t>
+  </si>
+  <si>
+    <t>images/lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>Olov Johansson</t>
+  </si>
+  <si>
+    <t>1960 CE</t>
+  </si>
+  <si>
+    <t>www.ericsahlstrom.se</t>
+  </si>
+  <si>
+    <t>images/eric.jpg</t>
+  </si>
+  <si>
+    <t>http://esitobo.org/eng/</t>
+  </si>
+  <si>
+    <t>Eric Sahlström-institutet</t>
+  </si>
+  <si>
+    <t>Eric Sahlström, from Göksby, begins rescuing the nyckelharpa from obscurity</t>
+  </si>
+  <si>
+    <t>Wood dates back to 1526 but was the instrument assembled later? We'll never know! This instrument is in the Zorn museum in Mora. Shaped more like a lute.</t>
+  </si>
+  <si>
+    <t>Vefsen harpa. Currently in Musik Museum in Stockholm.</t>
+  </si>
+  <si>
+    <t>Esseharpa, shaped more like a nyckelharpa than its predecessor, the Moraharpa</t>
+  </si>
+  <si>
+    <t>Kontrabasharpa! This was the type of nyckelharpa that Byss-Calle (1783-1847), one of the all-time greatest nyckelharpa players, used.</t>
+  </si>
+  <si>
+    <t>Silverbasharpa- plays best in C major. Invented and played the most in Tierp, aka the Tierpsharpa. Named for the use of a silver-wrapped gut string for the bass string to get more sound.</t>
+  </si>
+  <si>
+    <t>Schlüsselfideln- German word for Nyckelharpa</t>
+  </si>
+  <si>
+    <t>Sigtuna key! https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>Two angels with nyckelharpa at Tolfta church</t>
+  </si>
+  <si>
+    <t>public domain</t>
+  </si>
+  <si>
+    <t>American Nyckelharpa Association</t>
+  </si>
+  <si>
+    <t>1930 CE</t>
+  </si>
+  <si>
+    <t>August Bohlin wanted to play with fiddlers, so he made it so there were 3 rows of keys and fully chromatic.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
+  </si>
+  <si>
+    <t>images/bohlin.jpeg</t>
+  </si>
+  <si>
+    <t>Sandberg, Paul/Upplandsmuseet</t>
   </si>
 </sst>
 </file>
@@ -389,18 +449,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -731,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C19648A-7D51-4B77-BA95-465F033E890E}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,25 +829,25 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
         <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,16 +864,19 @@
         <v>18.568551200000002</v>
       </c>
       <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" t="s">
-        <v>87</v>
+      <c r="I2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +884,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>61.007080799999997</v>
@@ -816,24 +893,27 @@
         <v>14.482189999999999</v>
       </c>
       <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
         <v>78</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
+      <c r="I3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>65.845207099999996</v>
@@ -842,24 +922,27 @@
         <v>13.145485300000001</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>63.600692000000002</v>
@@ -868,16 +951,19 @@
         <v>22.788154500000001</v>
       </c>
       <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
         <v>79</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" t="s">
-        <v>89</v>
+      <c r="I5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -885,7 +971,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>59.833205100000001</v>
@@ -894,24 +980,27 @@
         <v>17.518364699999999</v>
       </c>
       <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
         <v>80</v>
       </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>59.612140799999999</v>
@@ -920,19 +1009,19 @@
         <v>17.688720199999999</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
+        <v>71</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -940,7 +1029,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>60.259325400000002</v>
@@ -949,24 +1038,27 @@
         <v>17.6540985</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>43.317990899999998</v>
@@ -975,19 +1067,19 @@
         <v>11.329836999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
         <v>91</v>
-      </c>
-      <c r="I9" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -995,36 +1087,36 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C10">
-        <v>60.347051299999997</v>
+        <v>60.357051300000002</v>
       </c>
       <c r="D10">
-        <v>17.484182700000002</v>
+        <v>17.4941827</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>52.143595900000001</v>
@@ -1033,27 +1125,27 @@
         <v>9.8746261000000004</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C12">
         <v>51.076749999999997</v>
@@ -1062,30 +1154,151 @@
         <v>13.632501599999999</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="I12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>60.347051299999997</v>
+      </c>
+      <c r="D13">
+        <v>17.484182700000002</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" t="s">
         <v>100</v>
       </c>
+      <c r="I13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>59.797174200000001</v>
+      </c>
+      <c r="D14">
+        <v>17.828809799999998</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>60.306415000000001</v>
+      </c>
+      <c r="D15">
+        <v>17.7290031</v>
+      </c>
+      <c r="E15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>60.434713700000003</v>
+      </c>
+      <c r="D16">
+        <v>17.773121499999998</v>
+      </c>
+      <c r="E16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" location="/media/File:Viola_a_chiavi_Siena_1408.jpg" xr:uid="{13338E98-F238-4A3B-AC5F-65948EC73BF5}"/>
-    <hyperlink ref="G8" r:id="rId2" xr:uid="{F6175E98-D11D-4443-959D-0FBAC7D03B22}"/>
-    <hyperlink ref="G10" r:id="rId3" xr:uid="{B23186D6-252A-4B93-99F7-350D60FAD10D}"/>
-    <hyperlink ref="G7" r:id="rId4" xr:uid="{8F61598F-DCFC-47D8-814E-765D1E3ABD12}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{B23186D6-252A-4B93-99F7-350D60FAD10D}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{8F61598F-DCFC-47D8-814E-765D1E3ABD12}"/>
+    <hyperlink ref="I15" r:id="rId4" xr:uid="{D903E0E2-55F0-4FE3-9145-7D7D150CDADC}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{F17BAB83-F487-4B2C-B3F5-33A282756CFF}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{7C81E384-367B-4916-9C3C-C806804FF5E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tried markdown to see if images would show there but nope
</commit_message>
<xml_diff>
--- a/NyckelharpaHistoryData.xlsx
+++ b/NyckelharpaHistoryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E229C2-B2D6-4E1B-863F-D0B4907C8B44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7C4C54-9895-4C11-836B-027E30B65531}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
@@ -287,124 +287,124 @@
     <t>images/Schluesselfidel.jpg</t>
   </si>
   <si>
+    <t>images/vefsen.png</t>
+  </si>
+  <si>
+    <t>Image Source</t>
+  </si>
+  <si>
+    <t>Magnus Holmström</t>
+  </si>
+  <si>
+    <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>images/sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>By User:pincopallino - Own work, Public Domain</t>
+  </si>
+  <si>
+    <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
+  </si>
+  <si>
+    <t>images/ESI.jpg</t>
+  </si>
+  <si>
+    <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
+  </si>
+  <si>
+    <t>Angel on a fresco on the ceiling of the Palazzo Pubblico (town hall) by Taddeo di Bartolo</t>
+  </si>
+  <si>
+    <t>1830 CE</t>
+  </si>
+  <si>
+    <t>https://olovjohansson.se/nyckelharpa/</t>
+  </si>
+  <si>
+    <t>1498 CE</t>
+  </si>
+  <si>
+    <t>Lagga church outside of Uppsala</t>
+  </si>
+  <si>
+    <t>images/Silverbasharpa.jpg</t>
+  </si>
+  <si>
+    <t>images/lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>Olov Johansson</t>
+  </si>
+  <si>
+    <t>1960 CE</t>
+  </si>
+  <si>
+    <t>www.ericsahlstrom.se</t>
+  </si>
+  <si>
+    <t>images/eric.jpg</t>
+  </si>
+  <si>
+    <t>http://esitobo.org/eng/</t>
+  </si>
+  <si>
+    <t>Eric Sahlström-institutet</t>
+  </si>
+  <si>
+    <t>Eric Sahlström, from Göksby, begins rescuing the nyckelharpa from obscurity</t>
+  </si>
+  <si>
+    <t>Wood dates back to 1526 but was the instrument assembled later? We'll never know! This instrument is in the Zorn museum in Mora. Shaped more like a lute.</t>
+  </si>
+  <si>
+    <t>Vefsen harpa. Currently in Musik Museum in Stockholm.</t>
+  </si>
+  <si>
+    <t>Esseharpa, shaped more like a nyckelharpa than its predecessor, the Moraharpa</t>
+  </si>
+  <si>
+    <t>Kontrabasharpa! This was the type of nyckelharpa that Byss-Calle (1783-1847), one of the all-time greatest nyckelharpa players, used.</t>
+  </si>
+  <si>
+    <t>Silverbasharpa- plays best in C major. Invented and played the most in Tierp, aka the Tierpsharpa. Named for the use of a silver-wrapped gut string for the bass string to get more sound.</t>
+  </si>
+  <si>
+    <t>Schlüsselfideln- German word for Nyckelharpa</t>
+  </si>
+  <si>
+    <t>Sigtuna key! https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>Two angels with nyckelharpa at Tolfta church</t>
+  </si>
+  <si>
+    <t>public domain</t>
+  </si>
+  <si>
+    <t>American Nyckelharpa Association</t>
+  </si>
+  <si>
+    <t>1930 CE</t>
+  </si>
+  <si>
+    <t>August Bohlin wanted to play with fiddlers, so he made it so there were 3 rows of keys and fully chromatic.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
+  </si>
+  <si>
+    <t>images/bohlin.jpeg</t>
+  </si>
+  <si>
+    <t>Sandberg, Paul/Upplandsmuseet</t>
+  </si>
+  <si>
     <t>images/Strohfiddel.jpg</t>
-  </si>
-  <si>
-    <t>images/vefsen.png</t>
-  </si>
-  <si>
-    <t>Image Source</t>
-  </si>
-  <si>
-    <t>Magnus Holmström</t>
-  </si>
-  <si>
-    <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
-  </si>
-  <si>
-    <t>images/sigtuna.jpg</t>
-  </si>
-  <si>
-    <t>Wikimedia Commons</t>
-  </si>
-  <si>
-    <t>By User:pincopallino - Own work, Public Domain</t>
-  </si>
-  <si>
-    <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
-  </si>
-  <si>
-    <t>images/ESI.jpg</t>
-  </si>
-  <si>
-    <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
-  </si>
-  <si>
-    <t>Angel on a fresco on the ceiling of the Palazzo Pubblico (town hall) by Taddeo di Bartolo</t>
-  </si>
-  <si>
-    <t>1830 CE</t>
-  </si>
-  <si>
-    <t>https://olovjohansson.se/nyckelharpa/</t>
-  </si>
-  <si>
-    <t>1498 CE</t>
-  </si>
-  <si>
-    <t>Lagga church outside of Uppsala</t>
-  </si>
-  <si>
-    <t>images/Silverbasharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/lagga-600.jpg</t>
-  </si>
-  <si>
-    <t>Olov Johansson</t>
-  </si>
-  <si>
-    <t>1960 CE</t>
-  </si>
-  <si>
-    <t>www.ericsahlstrom.se</t>
-  </si>
-  <si>
-    <t>images/eric.jpg</t>
-  </si>
-  <si>
-    <t>http://esitobo.org/eng/</t>
-  </si>
-  <si>
-    <t>Eric Sahlström-institutet</t>
-  </si>
-  <si>
-    <t>Eric Sahlström, from Göksby, begins rescuing the nyckelharpa from obscurity</t>
-  </si>
-  <si>
-    <t>Wood dates back to 1526 but was the instrument assembled later? We'll never know! This instrument is in the Zorn museum in Mora. Shaped more like a lute.</t>
-  </si>
-  <si>
-    <t>Vefsen harpa. Currently in Musik Museum in Stockholm.</t>
-  </si>
-  <si>
-    <t>Esseharpa, shaped more like a nyckelharpa than its predecessor, the Moraharpa</t>
-  </si>
-  <si>
-    <t>Kontrabasharpa! This was the type of nyckelharpa that Byss-Calle (1783-1847), one of the all-time greatest nyckelharpa players, used.</t>
-  </si>
-  <si>
-    <t>Silverbasharpa- plays best in C major. Invented and played the most in Tierp, aka the Tierpsharpa. Named for the use of a silver-wrapped gut string for the bass string to get more sound.</t>
-  </si>
-  <si>
-    <t>Schlüsselfideln- German word for Nyckelharpa</t>
-  </si>
-  <si>
-    <t>Sigtuna key! https://nyckelharpansforum.net/sigtunanyckel.htm</t>
-  </si>
-  <si>
-    <t>Two angels with nyckelharpa at Tolfta church</t>
-  </si>
-  <si>
-    <t>public domain</t>
-  </si>
-  <si>
-    <t>American Nyckelharpa Association</t>
-  </si>
-  <si>
-    <t>1930 CE</t>
-  </si>
-  <si>
-    <t>August Bohlin wanted to play with fiddlers, so he made it so there were 3 rows of keys and fully chromatic.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
-  </si>
-  <si>
-    <t>images/bohlin.jpeg</t>
-  </si>
-  <si>
-    <t>Sandberg, Paul/Upplandsmuseet</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
         <v>64</v>
@@ -867,7 +867,7 @@
         <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
@@ -876,7 +876,7 @@
         <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,16 +896,16 @@
         <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
         <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,16 +925,16 @@
         <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
@@ -963,7 +963,7 @@
         <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>49</v>
@@ -992,7 +992,7 @@
         <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1012,16 +1012,16 @@
         <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
         <v>88</v>
       </c>
-      <c r="H7" t="s">
-        <v>89</v>
-      </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1044,13 +1044,13 @@
         <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
         <v>106</v>
-      </c>
-      <c r="H8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
@@ -1079,7 +1079,7 @@
         <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>55</v>
@@ -1108,7 +1108,7 @@
         <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>58</v>
@@ -1137,7 +1137,7 @@
         <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,10 +1163,10 @@
         <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1183,19 +1183,19 @@
         <v>17.484182700000002</v>
       </c>
       <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" t="s">
         <v>96</v>
       </c>
-      <c r="F13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" t="s">
-        <v>97</v>
-      </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1212,19 +1212,19 @@
         <v>17.828809799999998</v>
       </c>
       <c r="E14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" t="s">
         <v>98</v>
       </c>
-      <c r="F14" t="s">
-        <v>99</v>
-      </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
         <v>101</v>
-      </c>
-      <c r="I14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,19 +1241,19 @@
         <v>17.7290031</v>
       </c>
       <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" t="s">
         <v>103</v>
       </c>
-      <c r="F15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>104</v>
       </c>
-      <c r="H15" t="s">
-        <v>105</v>
-      </c>
       <c r="I15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1270,19 +1270,19 @@
         <v>17.773121499999998</v>
       </c>
       <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s">
         <v>119</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>120</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>121</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>122</v>
-      </c>
-      <c r="I16" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
had to add a RemoteImage column because I can't get this to work with local images. Uploaded the images to my own site and linked to them from here.
</commit_message>
<xml_diff>
--- a/NyckelharpaHistoryData.xlsx
+++ b/NyckelharpaHistoryData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiadso\Documents\R\Nyckelharpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7C4C54-9895-4C11-836B-027E30B65531}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DC2E83-1C61-4FEA-AD26-D7F57DC3DC2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Geo" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
   <si>
     <t>InstrumentName</t>
   </si>
@@ -266,30 +266,6 @@
     <t>1619 CE</t>
   </si>
   <si>
-    <t>images/kallunge_carving.jpg</t>
-  </si>
-  <si>
-    <t>images/moraharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/esse_harpa.jpg</t>
-  </si>
-  <si>
-    <t>images/kontrabasharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/Viola_a_chiavi_Siena_1408.jpg</t>
-  </si>
-  <si>
-    <t>images/tolfta.jpg</t>
-  </si>
-  <si>
-    <t>images/Schluesselfidel.jpg</t>
-  </si>
-  <si>
-    <t>images/vefsen.png</t>
-  </si>
-  <si>
     <t>Image Source</t>
   </si>
   <si>
@@ -299,9 +275,6 @@
     <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
   </si>
   <si>
-    <t>images/sigtuna.jpg</t>
-  </si>
-  <si>
     <t>Wikimedia Commons</t>
   </si>
   <si>
@@ -311,9 +284,6 @@
     <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
   </si>
   <si>
-    <t>images/ESI.jpg</t>
-  </si>
-  <si>
     <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
   </si>
   <si>
@@ -332,12 +302,6 @@
     <t>Lagga church outside of Uppsala</t>
   </si>
   <si>
-    <t>images/Silverbasharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/lagga-600.jpg</t>
-  </si>
-  <si>
     <t>Olov Johansson</t>
   </si>
   <si>
@@ -347,9 +311,6 @@
     <t>www.ericsahlstrom.se</t>
   </si>
   <si>
-    <t>images/eric.jpg</t>
-  </si>
-  <si>
     <t>http://esitobo.org/eng/</t>
   </si>
   <si>
@@ -398,13 +359,100 @@
     <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
   </si>
   <si>
-    <t>images/bohlin.jpeg</t>
-  </si>
-  <si>
     <t>Sandberg, Paul/Upplandsmuseet</t>
   </si>
   <si>
-    <t>images/Strohfiddel.jpg</t>
+    <t>www/images/kallunge_carving.jpg</t>
+  </si>
+  <si>
+    <t>www/images/moraharpa.jpg</t>
+  </si>
+  <si>
+    <t>www/images/vefsen.png</t>
+  </si>
+  <si>
+    <t>www/images/esse_harpa.jpg</t>
+  </si>
+  <si>
+    <t>www/images/kontrabasharpa.jpg</t>
+  </si>
+  <si>
+    <t>www/images/sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>www/images/ESI.jpg</t>
+  </si>
+  <si>
+    <t>www/images/Viola_a_chiavi_Siena_1408.jpg</t>
+  </si>
+  <si>
+    <t>www/images/tolfta.jpg</t>
+  </si>
+  <si>
+    <t>www/images/Schluesselfidel.jpg</t>
+  </si>
+  <si>
+    <t>www/images/Strohfiddel.jpg</t>
+  </si>
+  <si>
+    <t>www/images/Silverbasharpa.jpg</t>
+  </si>
+  <si>
+    <t>www/images/lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>www/images/eric.jpg</t>
+  </si>
+  <si>
+    <t>www/images/bohlin.jpeg</t>
+  </si>
+  <si>
+    <t>RemoteImage</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Bohlin-1024x704.jpeg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/eric.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/esse_harpa.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/ESI.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/kallunge_carving.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/kontrabasharpa.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/moraharpa.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Schluesselfidel.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Silverbasharpa-1024x365.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Strohfiddel.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Vefsen.png</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/tolfta.jpg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/Viola_a_chiavi_Siena_1408.jpg</t>
   </si>
 </sst>
 </file>
@@ -805,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C19648A-7D51-4B77-BA95-465F033E890E}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,10 +866,11 @@
     <col min="6" max="6" width="39.7109375" customWidth="1"/>
     <col min="7" max="7" width="53.140625" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="10" max="10" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -841,16 +890,19 @@
         <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
         <v>64</v>
       </c>
       <c r="I1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -867,19 +919,22 @@
         <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -896,19 +951,22 @@
         <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -925,19 +983,22 @@
         <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="J4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -954,19 +1015,22 @@
         <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -983,19 +1047,22 @@
         <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1012,19 +1079,22 @@
         <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
       <c r="I7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1044,16 +1114,19 @@
         <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="I8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="J8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1070,19 +1143,22 @@
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" t="s">
         <v>81</v>
       </c>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1099,19 +1175,22 @@
         <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1128,19 +1207,22 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1163,13 +1245,16 @@
         <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="J12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1183,22 +1268,25 @@
         <v>17.484182700000002</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="I13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="J13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1212,22 +1300,25 @@
         <v>17.828809799999998</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="I14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1241,22 +1332,25 @@
         <v>17.7290031</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="I15" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1270,19 +1364,22 @@
         <v>17.773121499999998</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="H16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>125</v>
+      </c>
+      <c r="J16" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1390,7 @@
     <hyperlink ref="G9" r:id="rId1" location="/media/File:Viola_a_chiavi_Siena_1408.jpg" xr:uid="{13338E98-F238-4A3B-AC5F-65948EC73BF5}"/>
     <hyperlink ref="G10" r:id="rId2" xr:uid="{B23186D6-252A-4B93-99F7-350D60FAD10D}"/>
     <hyperlink ref="G7" r:id="rId3" xr:uid="{8F61598F-DCFC-47D8-814E-765D1E3ABD12}"/>
-    <hyperlink ref="I15" r:id="rId4" xr:uid="{D903E0E2-55F0-4FE3-9145-7D7D150CDADC}"/>
+    <hyperlink ref="J15" r:id="rId4" xr:uid="{D903E0E2-55F0-4FE3-9145-7D7D150CDADC}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{F17BAB83-F487-4B2C-B3F5-33A282756CFF}"/>
     <hyperlink ref="G3" r:id="rId6" xr:uid="{7C81E384-367B-4916-9C3C-C806804FF5E1}"/>
   </hyperlinks>

</xml_diff>